<commit_message>
Update omni-schema so that it parses Benchmark-001.yaml example
</commit_message>
<xml_diff>
--- a/project/excel/omni_schema.xlsx
+++ b/project/excel/omni_schema.xlsx
@@ -618,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,12 +629,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>path</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>path</t>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -686,7 +696,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>values</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add version, storage, and validator fields to the schema.
</commit_message>
<xml_diff>
--- a/project/excel/omni_schema.xlsx
+++ b/project/excel/omni_schema.xlsx
@@ -9,11 +9,12 @@
   <sheets>
     <sheet name="Benchmark" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Orchestrator" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Step" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Module" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="IOFile" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="InputCollection" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Parameter" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Validator" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Step" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Module" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="IOFile" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="InputCollection" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Parameter" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -419,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,30 +431,45 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>platform</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>storage</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>orchestrator</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>validator</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
         <is>
           <t>steps</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -501,6 +517,42 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>schema_url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -561,7 +613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -612,7 +664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -645,32 +697,6 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>entries</t>
         </is>
       </c>
     </row>
@@ -696,6 +722,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>entries</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>values</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Update omni-schema according to latest spec
</commit_message>
<xml_diff>
--- a/project/excel/omni_schema.xlsx
+++ b/project/excel/omni_schema.xlsx
@@ -8,13 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Benchmark" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Orchestrator" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Validator" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Step" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Module" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="IOFile" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="InputCollection" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Parameter" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Stage" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Module" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="IOFile" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="InputCollection" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Repository" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Parameter" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="SoftwareEnvironment" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>platform</t>
+          <t>benchmarker</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -446,30 +446,91 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>orchestrator</t>
+          <t>storage_api</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>validator</t>
+          <t>software_environments</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>steps</t>
+          <t>benchmark_yaml_spec</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>stages</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"S3"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>modules</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>inputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -480,7 +541,130 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>software_environment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>exclude</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>parameters</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>path</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>entries</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -497,206 +681,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>url</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>url</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>schema_url</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>initial</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>terminal</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>after</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>members</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>inputs</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>outputs</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>repo</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>exclude</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>parameters</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>path</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
+          <t>commit</t>
         </is>
       </c>
     </row>
@@ -722,7 +712,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>values</t>
         </is>
       </c>
     </row>
@@ -737,7 +727,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,7 +738,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>values</t>
+          <t>easyconfig</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>envmodule</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>conda</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>apptainer</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add software backend, document singularity URLs should be ORAS
</commit_message>
<xml_diff>
--- a/project/excel/omni_schema.xlsx
+++ b/project/excel/omni_schema.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,40 +441,45 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>software_backend</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>storage</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>storage_api</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>software_environments</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>benchmark_yaml_spec</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>stages</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -482,7 +487,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"S3"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add bucketname to schema
</commit_message>
<xml_diff>
--- a/project/excel/omni_schema.xlsx
+++ b/project/excel/omni_schema.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,30 +456,35 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>storage_bucket_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>software_environments</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>benchmark_yaml_spec</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>stages</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Include is_metric flag at module level
</commit_message>
<xml_diff>
--- a/project/excel/omni_schema.xlsx
+++ b/project/excel/omni_schema.xlsx
@@ -560,7 +560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -591,15 +591,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>is_metric</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Run make all and update CHANGELOG.md
</commit_message>
<xml_diff>
--- a/project/excel/omni_schema.xlsx
+++ b/project/excel/omni_schema.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Repository" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Parameter" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="SoftwareEnvironment" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="MetricCollector" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -788,4 +789,60 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>software_environment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>inputs</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add metric_collectors field to Benchmark
</commit_message>
<xml_diff>
--- a/project/excel/omni_schema.xlsx
+++ b/project/excel/omni_schema.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,20 +472,25 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>metric_collectors</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>stages</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>